<commit_message>
Todas las correccciones sin testeo
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/germanlopezpineda/Documents/Python/CargaAdmisible/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD967B48-1D82-6240-A7C1-09268ECB403D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC08720-0B11-3943-864C-4521B2BF9E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="4200" windowWidth="27200" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2180" yWindow="1560" windowWidth="33240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CargaAdmisible" sheetId="2" r:id="rId1"/>
+    <sheet name="CargaAdmisible_hundimiento" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>B=</t>
   </si>
@@ -111,9 +111,6 @@
     <t>prof plano cimentación=</t>
   </si>
   <si>
-    <t xml:space="preserve">Inclinación </t>
-  </si>
-  <si>
     <t>beta</t>
   </si>
   <si>
@@ -124,6 +121,42 @@
   </si>
   <si>
     <t>tg</t>
+  </si>
+  <si>
+    <t>HB=</t>
+  </si>
+  <si>
+    <t>N=</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>TandeltaL=</t>
+  </si>
+  <si>
+    <t>TandeltaB=</t>
+  </si>
+  <si>
+    <t>ic=</t>
+  </si>
+  <si>
+    <t>ig=</t>
+  </si>
+  <si>
+    <t>iq=</t>
+  </si>
+  <si>
+    <t>HL=</t>
+  </si>
+  <si>
+    <t>H=</t>
+  </si>
+  <si>
+    <t>Cargas</t>
+  </si>
+  <si>
+    <t>Inclinación apoyo</t>
   </si>
 </sst>
 </file>
@@ -162,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -172,6 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,15 +486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60474B96-411A-4D7E-8591-E087742093E8}">
-  <dimension ref="A3:N32"/>
+  <dimension ref="A3:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -491,13 +525,28 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -511,7 +560,26 @@
       </c>
       <c r="G5">
         <f>RADIANS(B5)</f>
-        <v>0.3490658503988659</v>
+        <v>0.43633231299858238</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <f>RADIANS(J5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <f>EXP(-2*K5*TAN($G$5))</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <f>1-SIN(2*K5)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="3">
+        <f>1-SIN(2*K5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -524,16 +592,75 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
+      <c r="J6" s="4">
+        <v>5</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6:K14" si="0">RADIANS(J6)</f>
+        <v>8.7266462599716474E-2</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" ref="L6:L14" si="1">EXP(-2*K6*TAN($G$5))</f>
+        <v>0.92183775684860947</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" ref="M6:M13" si="2">1-SIN(2*K6)</f>
+        <v>0.8263518223330697</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N13" si="3">1-SIN(2*K6)</f>
+        <v>0.8263518223330697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J7" s="4">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.84978484995167591</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.65797985667433134</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.65797985667433134</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
+      </c>
+      <c r="J8" s="4">
+        <v>15</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.78336375988338514</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -546,6 +673,25 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
+      <c r="J9" s="4">
+        <v>20</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.72213429120739236</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.35721239031346075</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.35721239031346075</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -557,6 +703,46 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="J10" s="4">
+        <v>25</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.43633231299858238</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.66569065515008308</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.23395555688102199</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.23395555688102199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J11" s="4">
+        <v>30</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.61365878029863385</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1339745962155614</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.1339745962155614</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -564,15 +750,55 @@
       </c>
       <c r="B12">
         <f>B8*B9</f>
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
+      <c r="J12" s="4">
+        <v>35</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.6108652381980153</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.56569383350094626</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="2"/>
+        <v>6.0307379214091683E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="3"/>
+        <v>6.0307379214091683E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J13" s="4">
+        <v>40</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.69813170079773179</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.52147793453760305</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.519224698779198E-2</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="3"/>
+        <v>1.519224698779198E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -584,152 +810,59 @@
         <f>RADIANS(B14)</f>
         <v>0.3490658503988659</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>29</v>
+      <c r="J14" s="4">
+        <v>45</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.48071804942018992</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" ref="M14" si="4">1-SIN(2*K14)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" ref="N14" si="5">1-SIN(2*K14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="4">
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <f>RADIANS(J15)</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
-        <f>EXP(-2*K15*TAN($G$5))</f>
-        <v>1</v>
-      </c>
-      <c r="M15" s="3">
-        <f>1-SIN(2*K15)</f>
-        <v>1</v>
-      </c>
-      <c r="N15" s="3">
-        <f>1-SIN(2*K15)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="2">
-        <f>(B17-1)/TAN(G5)</f>
-        <v>14.834711777931204</v>
-      </c>
-      <c r="J16" s="4">
-        <v>5</v>
-      </c>
-      <c r="K16" s="3">
-        <f t="shared" ref="K16:K24" si="0">RADIANS(J16)</f>
-        <v>8.7266462599716474E-2</v>
-      </c>
-      <c r="L16" s="3">
-        <f t="shared" ref="L16:L24" si="1">EXP(-2*K16*TAN($G$5))</f>
-        <v>0.93845085512341997</v>
-      </c>
-      <c r="M16" s="3">
-        <f t="shared" ref="M16:M23" si="2">1-SIN(2*K16)</f>
-        <v>0.8263518223330697</v>
-      </c>
-      <c r="N16" s="3">
-        <f t="shared" ref="N16:N23" si="3">1-SIN(2*K16)</f>
-        <v>0.8263518223330697</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <f>IF(B5=0,PI()+2,(B17-1)/TAN(G5))</f>
+        <v>20.720531219083689</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <f>((1+SIN(G5))/(1-SIN(G5)))*EXP(PI()*TAN(G5))</f>
-        <v>6.3993935210852113</v>
-      </c>
-      <c r="J17" s="4">
-        <v>10</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" si="0"/>
-        <v>0.17453292519943295</v>
-      </c>
-      <c r="L17" s="3">
-        <f t="shared" si="1"/>
-        <v>0.88069000748187809</v>
-      </c>
-      <c r="M17" s="3">
-        <f t="shared" si="2"/>
-        <v>0.65797985667433134</v>
-      </c>
-      <c r="N17" s="3">
-        <f t="shared" si="3"/>
-        <v>0.65797985667433134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10.662142388498452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2">
         <f>1.5*(B17-1)*TAN(G5)</f>
-        <v>2.9478277871471992</v>
-      </c>
-      <c r="J18" s="4">
-        <v>15</v>
-      </c>
-      <c r="K18" s="3">
-        <f t="shared" si="0"/>
-        <v>0.26179938779914941</v>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="1"/>
-        <v>0.8264842906200196</v>
-      </c>
-      <c r="M18" s="3">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="N18" s="3">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J19" s="4">
-        <v>20</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.3490658503988659</v>
-      </c>
-      <c r="L19" s="3">
-        <f t="shared" si="1"/>
-        <v>0.77561488927843047</v>
-      </c>
-      <c r="M19" s="3">
-        <f t="shared" si="2"/>
-        <v>0.35721239031346075</v>
-      </c>
-      <c r="N19" s="3">
-        <f t="shared" si="3"/>
-        <v>0.35721239031346075</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>6.7582964849112868</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -737,55 +870,17 @@
         <f>1+0.2*B3/B4</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="J20" s="4">
-        <v>25</v>
-      </c>
-      <c r="K20" s="3">
-        <f t="shared" si="0"/>
-        <v>0.43633231299858238</v>
-      </c>
-      <c r="L20" s="3">
-        <f t="shared" si="1"/>
-        <v>0.72787645608979978</v>
-      </c>
-      <c r="M20" s="3">
-        <f t="shared" si="2"/>
-        <v>0.23395555688102199</v>
-      </c>
-      <c r="N20" s="3">
-        <f t="shared" si="3"/>
-        <v>0.23395555688102199</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="2">
         <f>1+1.5*TAN(RADIANS(B5))*B3/B4</f>
-        <v>1.4367642811194428</v>
-      </c>
-      <c r="J21" s="4">
-        <v>30</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" si="0"/>
-        <v>0.52359877559829882</v>
-      </c>
-      <c r="L21" s="3">
-        <f t="shared" si="1"/>
-        <v>0.68307628264167697</v>
-      </c>
-      <c r="M21" s="3">
-        <f t="shared" si="2"/>
-        <v>0.1339745962155614</v>
-      </c>
-      <c r="N21" s="3">
-        <f t="shared" si="3"/>
-        <v>0.1339745962155614</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+        <v>1.5595691897859982</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -793,94 +888,144 @@
         <f>1-0.3*B3/B4</f>
         <v>0.76</v>
       </c>
-      <c r="J22" s="4">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="5">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2">
+        <f>SQRT(B27^2+B28^2)</f>
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2">
+        <f>B27/B26</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <f>B28/B26</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2">
+        <f>IF(B5=0,0.5*(1+SQRT(1-B29/(B3*B4*B6))),(B36*B17-1)/(B17-1))</f>
+        <v>0.75723072263332802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="3">
-        <f t="shared" si="0"/>
-        <v>0.6108652381980153</v>
-      </c>
-      <c r="L22" s="3">
-        <f t="shared" si="1"/>
-        <v>0.64103352155960869</v>
-      </c>
-      <c r="M22" s="3">
-        <f t="shared" si="2"/>
-        <v>6.0307379214091683E-2</v>
-      </c>
-      <c r="N22" s="3">
-        <f t="shared" si="3"/>
-        <v>6.0307379214091683E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J23" s="4">
-        <v>40</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.69813170079773179</v>
-      </c>
-      <c r="L23" s="3">
-        <f t="shared" si="1"/>
-        <v>0.60157845647039199</v>
-      </c>
-      <c r="M23" s="3">
-        <f t="shared" si="2"/>
-        <v>1.519224698779198E-2</v>
-      </c>
-      <c r="N23" s="3">
-        <f t="shared" si="3"/>
-        <v>1.519224698779198E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J24" s="4">
-        <v>45</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="0"/>
-        <v>0.78539816339744828</v>
-      </c>
-      <c r="L24" s="3">
-        <f t="shared" si="1"/>
-        <v>0.56455181689846634</v>
-      </c>
-      <c r="M24" s="3">
-        <f t="shared" ref="M24" si="4">1-SIN(2*K24)</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="3">
-        <f t="shared" ref="N24" si="5">1-SIN(2*K24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B35" s="2">
+        <f>(1-0.7*B31)^3*(1-B32)</f>
+        <v>0.6971094000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <f>(1-B31)*(1-B32)</f>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="2">
-        <f>B6*B16*B20+B12*B17*B21+0.5*B3*B10*B18*B22</f>
-        <v>377.90850132677906</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B39" s="2">
+        <f>B6*B16*B20*B34+B12*B17*B21*B35+0.5*B3*B10*B18*B22*B36</f>
+        <v>567.09832386968333</v>
+      </c>
+      <c r="C39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="2">
-        <f>B26/3</f>
-        <v>125.96950044225969</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B40" s="2">
+        <f>B39/3</f>
+        <v>189.03277462322777</v>
+      </c>
+      <c r="C40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>